<commit_message>
Add changes in our data from 2010-2012 regarding publications
</commit_message>
<xml_diff>
--- a/preprocessing/dotacie_pre/dotacie_nase_2010.xlsx
+++ b/preprocessing/dotacie_pre/dotacie_nase_2010.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Desktop\school\pridav\project\preprocessing\dotacie_pre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA9B54B-5C70-4A22-A1BC-168D3D008E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D6D29F-AD73-4038-88A1-490E2924AD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>studenti-denni</t>
   </si>
   <si>
-    <t>publikacie</t>
-  </si>
-  <si>
     <t>absolventi</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>UJS</t>
+  </si>
+  <si>
+    <t>publikácie</t>
   </si>
 </sst>
 </file>
@@ -143,9 +143,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;Sk&quot;_-;\-* #,##0.00\ &quot;Sk&quot;_-;_-* &quot;-&quot;??\ &quot;Sk&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _S_k_-;\-* #,##0.00\ _S_k_-;_-* &quot;-&quot;??\ _S_k_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;Sk&quot;_-;\-* #,##0.00\ &quot;Sk&quot;_-;_-* &quot;-&quot;??\ &quot;Sk&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _S_k_-;\-* #,##0.00\ _S_k_-;_-* &quot;-&quot;??\ _S_k_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -846,7 +846,7 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -856,7 +856,7 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -922,8 +922,8 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -960,8 +960,8 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="2" xr:uid="{40B71722-B102-4EE4-AEED-F6658C05C7C5}"/>
@@ -1306,7 +1306,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L21"/>
+      <selection activeCell="O2" sqref="O2:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1320,11 +1320,11 @@
     <col min="8" max="8" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1371,12 +1371,12 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>76955994</v>
@@ -1405,26 +1405,25 @@
       <c r="J2" s="16">
         <v>21706</v>
       </c>
-      <c r="K2">
-        <f>SUM(E24:H24)</f>
-        <v>14595</v>
-      </c>
-      <c r="L2" s="34">
+      <c r="K2" s="34">
         <v>19830.859219193466</v>
       </c>
-      <c r="M2" s="28">
+      <c r="L2" s="28">
         <v>11012</v>
       </c>
-      <c r="N2" s="30">
+      <c r="M2" s="30">
         <v>10004</v>
       </c>
-      <c r="O2" s="32">
+      <c r="N2" s="32">
         <v>793216</v>
+      </c>
+      <c r="O2">
+        <v>19.590538076794108</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>22020879</v>
@@ -1453,26 +1452,25 @@
       <c r="J3" s="16">
         <v>7269</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K21" si="0">SUM(E25:H25)</f>
-        <v>4263</v>
-      </c>
-      <c r="L3" s="34">
+      <c r="K3" s="34">
         <v>5279.8687195517759</v>
       </c>
-      <c r="M3" s="27">
+      <c r="L3" s="27">
         <v>1776</v>
       </c>
-      <c r="N3" s="30">
+      <c r="M3" s="30">
         <v>1781</v>
       </c>
-      <c r="O3" s="32">
+      <c r="N3" s="32">
         <v>127648</v>
+      </c>
+      <c r="O3">
+        <v>6.5998680685037794</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>17434872</v>
@@ -1501,26 +1499,25 @@
       <c r="J4" s="16">
         <v>7409</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>4519</v>
-      </c>
-      <c r="L4" s="34">
+      <c r="K4" s="34">
         <v>6889.1434796096637</v>
       </c>
-      <c r="M4" s="27">
+      <c r="L4" s="27">
         <v>1921</v>
       </c>
-      <c r="N4" s="30">
+      <c r="M4" s="30">
         <v>2007</v>
       </c>
-      <c r="O4" s="32">
+      <c r="N4" s="32">
         <v>158288</v>
+      </c>
+      <c r="O4">
+        <v>5.3458825709168263</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>7484225</v>
@@ -1549,26 +1546,25 @@
       <c r="J5" s="16">
         <v>5334</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>1137</v>
-      </c>
-      <c r="L5" s="34">
+      <c r="K5" s="34">
         <v>3734.0531821762606</v>
       </c>
-      <c r="M5" s="27">
+      <c r="L5" s="27">
         <v>224</v>
       </c>
-      <c r="N5" s="30">
+      <c r="M5" s="30">
         <v>224</v>
       </c>
-      <c r="O5" s="32">
+      <c r="N5" s="32">
         <v>14336</v>
+      </c>
+      <c r="O5">
+        <v>1.5498206170361948</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>8791849</v>
@@ -1597,26 +1593,25 @@
       <c r="J6" s="16">
         <v>1464</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>1851</v>
-      </c>
-      <c r="L6" s="34">
+      <c r="K6" s="34">
         <v>1266.8732103753434</v>
       </c>
-      <c r="M6" s="27">
+      <c r="L6" s="27">
         <v>899</v>
       </c>
-      <c r="N6" s="30">
+      <c r="M6" s="30">
         <v>775</v>
       </c>
-      <c r="O6" s="32">
+      <c r="N6" s="32">
         <v>41744</v>
+      </c>
+      <c r="O6">
+        <v>2.2922645513725421</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>19188933</v>
@@ -1645,26 +1640,25 @@
       <c r="J7" s="16">
         <v>8159</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>5214</v>
-      </c>
-      <c r="L7" s="34">
+      <c r="K7" s="34">
         <v>8024.344105969114</v>
       </c>
-      <c r="M7" s="27">
+      <c r="L7" s="27">
         <v>1597</v>
       </c>
-      <c r="N7" s="30">
+      <c r="M7" s="30">
         <v>1566</v>
       </c>
-      <c r="O7" s="32">
+      <c r="N7" s="32">
         <v>125280</v>
+      </c>
+      <c r="O7">
+        <v>7.0070381926300049</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>19076191</v>
@@ -1693,26 +1687,25 @@
       <c r="J8" s="16">
         <v>8380</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>5807</v>
-      </c>
-      <c r="L8" s="34">
+      <c r="K8" s="34">
         <v>7865.6548800090522</v>
       </c>
-      <c r="M8" s="27">
+      <c r="L8" s="27">
         <v>2434</v>
       </c>
-      <c r="N8" s="30">
+      <c r="M8" s="30">
         <v>2288</v>
       </c>
-      <c r="O8" s="32">
+      <c r="N8" s="32">
         <v>161280</v>
+      </c>
+      <c r="O8">
+        <v>7.4241506020518795</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>10564304</v>
@@ -1741,20 +1734,19 @@
       <c r="J9" s="16">
         <v>5191</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>2264</v>
-      </c>
-      <c r="L9" s="34">
+      <c r="K9" s="34">
         <v>3432.0148803169623</v>
       </c>
-      <c r="M9" s="27"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="32"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="32"/>
+      <c r="O9">
+        <v>3.1582135755131864</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
         <v>57204228</v>
@@ -1783,26 +1775,25 @@
       <c r="J10" s="16">
         <v>16882</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>12143</v>
-      </c>
-      <c r="L10" s="34">
+      <c r="K10" s="34">
         <v>15370.508506812526</v>
       </c>
-      <c r="M10" s="27">
+      <c r="L10" s="27">
         <v>8556</v>
       </c>
-      <c r="N10" s="30">
+      <c r="M10" s="30">
         <v>6592</v>
       </c>
-      <c r="O10" s="32">
+      <c r="N10" s="32">
         <v>523520</v>
+      </c>
+      <c r="O10">
+        <v>13.438374117585594</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>39751109</v>
@@ -1831,26 +1822,25 @@
       <c r="J11" s="16">
         <v>13626</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>8807</v>
-      </c>
-      <c r="L11" s="34">
+      <c r="K11" s="34">
         <v>11259.295327077911</v>
       </c>
-      <c r="M11" s="27">
+      <c r="L11" s="27">
         <v>4984</v>
       </c>
-      <c r="N11" s="30">
+      <c r="M11" s="30">
         <v>5986</v>
       </c>
-      <c r="O11" s="32">
+      <c r="N11" s="32">
         <v>396032</v>
+      </c>
+      <c r="O11">
+        <v>7.235628020010898</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>27692163</v>
@@ -1879,26 +1869,25 @@
       <c r="J12" s="16">
         <v>9288</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>6115</v>
-      </c>
-      <c r="L12" s="34">
+      <c r="K12" s="34">
         <v>8599.5582053605558</v>
       </c>
-      <c r="M12" s="27">
+      <c r="L12" s="27">
         <v>5007</v>
       </c>
-      <c r="N12" s="30">
+      <c r="M12" s="30">
         <v>4502</v>
       </c>
-      <c r="O12" s="32">
+      <c r="N12" s="32">
         <v>355120</v>
+      </c>
+      <c r="O12">
+        <v>4.2576443926396825</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>8393123</v>
@@ -1927,26 +1916,25 @@
       <c r="J13" s="16">
         <v>4139</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>1952</v>
-      </c>
-      <c r="L13" s="34">
+      <c r="K13" s="34">
         <v>4536.774043663675</v>
       </c>
-      <c r="M13" s="27">
+      <c r="L13" s="27">
         <v>320</v>
       </c>
-      <c r="N13" s="30">
+      <c r="M13" s="30">
         <v>216</v>
       </c>
-      <c r="O13" s="32">
+      <c r="N13" s="32">
         <v>12000</v>
+      </c>
+      <c r="O13">
+        <v>1.764222352832153</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1">
         <v>21532693</v>
@@ -1975,26 +1963,25 @@
       <c r="J14" s="16">
         <v>10704</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>5427</v>
-      </c>
-      <c r="L14" s="34">
+      <c r="K14" s="34">
         <v>9413.163624550647</v>
       </c>
-      <c r="M14" s="27">
+      <c r="L14" s="27">
         <v>3480</v>
       </c>
-      <c r="N14" s="30">
+      <c r="M14" s="30">
         <v>3455</v>
       </c>
-      <c r="O14" s="32">
+      <c r="N14" s="32">
         <v>250496</v>
+      </c>
+      <c r="O14">
+        <v>5.9748798690097287</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1">
         <v>19597966</v>
@@ -2023,26 +2010,25 @@
       <c r="J15" s="16">
         <v>6953</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>4355</v>
-      </c>
-      <c r="L15" s="34">
+      <c r="K15" s="34">
         <v>7093.5864926509385</v>
       </c>
-      <c r="M15" s="27">
+      <c r="L15" s="27">
         <v>3028</v>
       </c>
-      <c r="N15" s="30">
+      <c r="M15" s="30">
         <v>2713</v>
       </c>
-      <c r="O15" s="32">
+      <c r="N15" s="32">
         <v>198416</v>
+      </c>
+      <c r="O15">
+        <v>4.4938677679046348</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>11237065</v>
@@ -2071,26 +2057,25 @@
       <c r="J16" s="16">
         <v>3302</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>2487</v>
-      </c>
-      <c r="L16" s="34">
+      <c r="K16" s="34">
         <v>3297.9799665098481</v>
       </c>
-      <c r="M16" s="27">
+      <c r="L16" s="27">
         <v>1524</v>
       </c>
-      <c r="N16" s="30">
+      <c r="M16" s="30">
         <v>1415</v>
       </c>
-      <c r="O16" s="32">
+      <c r="N16" s="32">
         <v>85328</v>
+      </c>
+      <c r="O16">
+        <v>3.0598974932277403</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>5327725</v>
@@ -2119,24 +2104,23 @@
       <c r="J17" s="16">
         <v>1009</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>116</v>
-      </c>
-      <c r="L17" s="34">
+      <c r="K17" s="34">
         <v>1991.5045976910571</v>
       </c>
-      <c r="M17" s="27"/>
-      <c r="N17" s="30">
+      <c r="L17" s="27"/>
+      <c r="M17" s="30">
         <v>0</v>
       </c>
-      <c r="O17" s="32">
+      <c r="N17" s="32">
         <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0.35174435312565971</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>4209279</v>
@@ -2165,24 +2149,23 @@
       <c r="J18" s="16">
         <v>675</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>201</v>
-      </c>
-      <c r="L18" s="34">
+      <c r="K18" s="34">
         <v>1353.5060000000003</v>
       </c>
-      <c r="M18" s="27"/>
-      <c r="N18" s="30">
+      <c r="L18" s="27"/>
+      <c r="M18" s="30">
         <v>0</v>
       </c>
-      <c r="O18" s="32">
+      <c r="N18" s="32">
         <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0.37421537687695766</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1">
         <v>2993615</v>
@@ -2211,26 +2194,25 @@
       <c r="J19" s="16">
         <v>615</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>94</v>
-      </c>
-      <c r="L19" s="34">
+      <c r="K19" s="34">
         <v>1177.2154681763095</v>
       </c>
-      <c r="M19" s="27">
+      <c r="L19" s="27">
         <v>201</v>
       </c>
-      <c r="N19" s="30">
+      <c r="M19" s="30">
         <v>156</v>
       </c>
-      <c r="O19" s="32">
+      <c r="N19" s="32">
         <v>9984</v>
+      </c>
+      <c r="O19">
+        <v>0.27844371999703177</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>12150310</v>
@@ -2259,26 +2241,25 @@
       <c r="J20" s="16">
         <v>4922</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>3179</v>
-      </c>
-      <c r="L20" s="34">
+      <c r="K20" s="34">
         <v>6230.7167176660532</v>
       </c>
-      <c r="M20" s="27">
+      <c r="L20" s="27">
         <v>699</v>
       </c>
-      <c r="N20" s="30">
+      <c r="M20" s="30">
         <v>590</v>
       </c>
-      <c r="O20" s="32">
+      <c r="N20" s="32">
         <v>35152</v>
+      </c>
+      <c r="O20">
+        <v>5.0371710899626034</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1">
         <v>2588024</v>
@@ -2307,21 +2288,20 @@
       <c r="J21" s="17">
         <v>1480</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>586</v>
-      </c>
-      <c r="L21" s="35">
+      <c r="K21" s="35">
         <v>1122.011640144927</v>
       </c>
-      <c r="M21" s="29">
+      <c r="L21" s="29">
         <v>513</v>
       </c>
-      <c r="N21" s="31">
+      <c r="M21" s="31">
         <v>477</v>
       </c>
-      <c r="O21" s="33">
+      <c r="N21" s="33">
         <v>38160</v>
+      </c>
+      <c r="O21">
+        <v>0.76613519200879343</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>

</xml_diff>